<commit_message>
fixed recap data. Data entry error on two birds
</commit_message>
<xml_diff>
--- a/data/2025/2025_MCGO_banding_data_recaps.xlsx
+++ b/data/2025/2025_MCGO_banding_data_recaps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/randall_friendly_fws_gov1/Documents/Desktop/cackler/data/2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfriendly\OneDrive - DOI\Desktop\cackler\data\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{ADEABFF4-6724-454B-AEE6-62B5A8FA84F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F1FCEC8-5ACD-43B3-BFE2-A5F8332280A4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3145AD85-EDCF-4D31-AD80-2C08EB6A2B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59145" yWindow="6285" windowWidth="25875" windowHeight="12915" xr2:uid="{3E845492-6596-40E8-B180-46107DEDDECF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{3E845492-6596-40E8-B180-46107DEDDECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,8 +500,8 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37:I40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1837,7 +1837,7 @@
         <v>14</v>
       </c>
       <c r="C33">
-        <v>2477</v>
+        <v>2497</v>
       </c>
       <c r="D33">
         <v>39291</v>

</xml_diff>